<commit_message>
Final commit for Part 1 of Traffic Simulator
</commit_message>
<xml_diff>
--- a/Results/simulation_results_exp.xlsx
+++ b/Results/simulation_results_exp.xlsx
@@ -5,22 +5,35 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Curso\RTEL\rtel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Curso\RTEL\rtel\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A462F777-95CC-482C-9D32-0A800260FC41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2480506C-CB0B-43B8-A0ED-45E6F5987344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>Total Calls</t>
   </si>
@@ -38,6 +51,9 @@
   </si>
   <si>
     <t>Target</t>
+  </si>
+  <si>
+    <t>Deviation</t>
   </si>
 </sst>
 </file>
@@ -91,16 +107,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -129,20 +160,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -156,11 +173,1091 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$J$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Deviation</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="22225" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$H$6:$H$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1250</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7500</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$J$6:$J$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>2.5090820259656976E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.3716153199768182E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.2531702039741714E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0275307309180497E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.8561322039811219E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.4482439799630162E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.7316623457271989E-5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.4372603887041202E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.2022664336377165E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-42BE-4D6B-8FDD-2E8C7B38B96F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1020365088"/>
+        <c:axId val="1020363648"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$H$5</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Total Calls</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$H$6:$H$14</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="9"/>
+                      <c:pt idx="0">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>125</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>250</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>500</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>1250</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>2500</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>5000</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>7500</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>10000</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$H$6:$H$14</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="9"/>
+                      <c:pt idx="0">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>125</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>250</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>500</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>1250</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>2500</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>5000</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>7500</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>10000</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000000-42BE-4D6B-8FDD-2E8C7B38B96F}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+          </c:ext>
+        </c:extLst>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1020365088"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1020363648"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1020363648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0E+00" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1020365088"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>601980</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>179070</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>297180</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>179070</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04BA93F4-F14D-9DB4-9BD9-610B0D6C8BF3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C89825BA-2D67-4821-A3BB-811B6F08CD0B}" name="Table1" displayName="Table1" ref="A1:F28" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" tableBorderDxfId="2">
-  <autoFilter ref="A1:F28" xr:uid="{C89825BA-2D67-4821-A3BB-811B6F08CD0B}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F28">
-    <sortCondition ref="D1:D28"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C89825BA-2D67-4821-A3BB-811B6F08CD0B}" name="Table1" displayName="Table1" ref="A1:F46" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
+  <autoFilter ref="A1:F46" xr:uid="{C89825BA-2D67-4821-A3BB-811B6F08CD0B}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F46">
+    <sortCondition ref="A1:A46"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{1F3F819B-2446-4038-B067-DAD01FB931E0}" name="Total Calls"/>
@@ -459,10 +1556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -474,7 +1571,7 @@
     <col min="5" max="5" width="14.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -494,7 +1591,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>50</v>
       </c>
@@ -514,29 +1611,29 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>500</v>
+        <v>50</v>
       </c>
       <c r="B3">
-        <v>356</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>0.71199999999999997</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>0.1860307443971965</v>
+        <v>0.2441999009867436</v>
       </c>
       <c r="E3">
+        <v>100</v>
+      </c>
+      <c r="F3">
         <v>50</v>
       </c>
-      <c r="F3">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>250</v>
+        <v>50</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -545,238 +1642,343 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>0.18968826131299019</v>
+        <v>0.20246057617065999</v>
       </c>
       <c r="E4">
         <v>200</v>
       </c>
       <c r="F4">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>250</v>
+        <v>50</v>
       </c>
       <c r="B5">
-        <v>147</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>0.58799999999999997</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>0.19351561581714549</v>
+        <v>0.223171649737475</v>
       </c>
       <c r="E5">
+        <v>350</v>
+      </c>
+      <c r="F5">
         <v>50</v>
       </c>
-      <c r="F5">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
+        <v>50</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0.16945842589165169</v>
+      </c>
+      <c r="E6">
         <v>500</v>
       </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0.19622981049565191</v>
-      </c>
-      <c r="E6">
-        <v>100</v>
-      </c>
       <c r="F6">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+      <c r="H6">
+        <v>50</v>
+      </c>
+      <c r="I6">
+        <f>AVERAGE(D2:D6)</f>
+        <v>0.19749091797403431</v>
+      </c>
+      <c r="J6" s="2">
+        <f>ABS(0.2-I6)</f>
+        <v>2.5090820259656976E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>7500</v>
+        <v>125</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>74</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>0.59199999999999997</v>
       </c>
       <c r="D7">
-        <v>0.19706118521253521</v>
+        <v>0.2079526988098267</v>
       </c>
       <c r="E7">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="F7">
-        <v>7500</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+      <c r="H7">
+        <v>125</v>
+      </c>
+      <c r="I7">
+        <f>AVERAGE(D7:D11)</f>
+        <v>0.20437161531997683</v>
+      </c>
+      <c r="J7" s="2">
+        <f t="shared" ref="J7:J14" si="0">ABS(0.2-I7)</f>
+        <v>4.3716153199768182E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>7500</v>
+        <v>125</v>
       </c>
       <c r="B8">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C8">
-        <v>6.6666666666666664E-4</v>
+        <v>2.4E-2</v>
       </c>
       <c r="D8">
-        <v>0.19711089904670601</v>
+        <v>0.23124964311832219</v>
       </c>
       <c r="E8">
         <v>100</v>
       </c>
       <c r="F8">
-        <v>7500</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+      <c r="H8">
+        <v>250</v>
+      </c>
+      <c r="I8">
+        <f>AVERAGE(D12:D16)</f>
+        <v>0.19574682979602584</v>
+      </c>
+      <c r="J8" s="2">
+        <f t="shared" si="0"/>
+        <v>4.2531702039741714E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
+        <v>125</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0.2033428866265182</v>
+      </c>
+      <c r="E9">
+        <v>200</v>
+      </c>
+      <c r="F9">
+        <v>125</v>
+      </c>
+      <c r="H9">
+        <v>500</v>
+      </c>
+      <c r="I9">
+        <f>AVERAGE(D17:D21)</f>
+        <v>0.20402753073091806</v>
+      </c>
+      <c r="J9" s="2">
+        <f t="shared" si="0"/>
+        <v>4.0275307309180497E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>125</v>
+      </c>
+      <c r="B10">
+        <v>102</v>
+      </c>
+      <c r="C10">
+        <v>0.81599999999999995</v>
+      </c>
+      <c r="D10">
+        <v>0.1797336112194329</v>
+      </c>
+      <c r="E10">
+        <v>350</v>
+      </c>
+      <c r="F10">
+        <v>125</v>
+      </c>
+      <c r="H10">
+        <v>1250</v>
+      </c>
+      <c r="I10">
+        <f>AVERAGE(D22:D26)</f>
+        <v>0.20385613220398113</v>
+      </c>
+      <c r="J10" s="2">
+        <f t="shared" si="0"/>
+        <v>3.8561322039811219E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>125</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0.19957923682578421</v>
+      </c>
+      <c r="E11">
+        <v>500</v>
+      </c>
+      <c r="F11">
+        <v>125</v>
+      </c>
+      <c r="H11">
+        <v>2500</v>
+      </c>
+      <c r="I11">
+        <f>AVERAGE(D27:D31)</f>
+        <v>0.20244824397996303</v>
+      </c>
+      <c r="J11" s="2">
+        <f t="shared" si="0"/>
+        <v>2.4482439799630162E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12">
         <v>250</v>
       </c>
-      <c r="B9">
-        <v>100</v>
-      </c>
-      <c r="C9">
-        <v>0.4</v>
-      </c>
-      <c r="D9">
-        <v>0.1977450689729946</v>
-      </c>
-      <c r="E9">
-        <v>100</v>
-      </c>
-      <c r="F9">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>10000</v>
-      </c>
-      <c r="B10">
-        <v>2536</v>
-      </c>
-      <c r="C10">
-        <v>0.25359999999999999</v>
-      </c>
-      <c r="D10">
-        <v>0.19778613638600959</v>
-      </c>
-      <c r="E10">
-        <v>50</v>
-      </c>
-      <c r="F10">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>10000</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0.19817352595832419</v>
-      </c>
-      <c r="E11">
-        <v>100</v>
-      </c>
-      <c r="F11">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>2500</v>
-      </c>
       <c r="B12">
-        <v>1606</v>
+        <v>147</v>
       </c>
       <c r="C12">
-        <v>0.64239999999999997</v>
+        <v>0.58799999999999997</v>
       </c>
       <c r="D12">
-        <v>0.19902327845823481</v>
+        <v>0.19351561581714549</v>
       </c>
       <c r="E12">
         <v>50</v>
       </c>
       <c r="F12">
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+        <v>250</v>
+      </c>
+      <c r="H12">
+        <v>5000</v>
+      </c>
+      <c r="I12">
+        <f>AVERAGE(D32:D36)</f>
+        <v>0.20009731662345728</v>
+      </c>
+      <c r="J12" s="2">
+        <f t="shared" si="0"/>
+        <v>9.7316623457271989E-5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>5000</v>
+        <v>250</v>
       </c>
       <c r="B13">
-        <v>3865</v>
+        <v>100</v>
       </c>
       <c r="C13">
-        <v>0.77300000000000002</v>
+        <v>0.4</v>
       </c>
       <c r="D13">
-        <v>0.19916207111113179</v>
+        <v>0.1977450689729946</v>
       </c>
       <c r="E13">
+        <v>100</v>
+      </c>
+      <c r="F13">
+        <v>250</v>
+      </c>
+      <c r="H13">
+        <v>7500</v>
+      </c>
+      <c r="I13">
+        <f>AVERAGE(D37:D41)</f>
+        <v>0.19856273961129589</v>
+      </c>
+      <c r="J13" s="2">
+        <f t="shared" si="0"/>
+        <v>1.4372603887041202E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>250</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0.18968826131299019</v>
+      </c>
+      <c r="E14">
         <v>200</v>
       </c>
-      <c r="F13">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>1250</v>
-      </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>0.19976847983663551</v>
-      </c>
-      <c r="E14">
-        <v>100</v>
-      </c>
       <c r="F14">
-        <v>1250</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+        <v>250</v>
+      </c>
+      <c r="H14">
+        <v>10000</v>
+      </c>
+      <c r="I14">
+        <f>AVERAGE(D42:D46)</f>
+        <v>0.19879773356636229</v>
+      </c>
+      <c r="J14" s="2">
+        <f t="shared" si="0"/>
+        <v>1.2022664336377165E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>7500</v>
+        <v>250</v>
       </c>
       <c r="B15">
-        <v>776</v>
+        <v>72</v>
       </c>
       <c r="C15">
-        <v>0.10346666666666671</v>
+        <v>0.28799999999999998</v>
       </c>
       <c r="D15">
-        <v>0.19978617109152219</v>
+        <v>0.20397369908704149</v>
       </c>
       <c r="E15">
-        <v>50</v>
+        <v>350</v>
       </c>
       <c r="F15">
-        <v>7500</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>10000</v>
+        <v>250</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -785,38 +1987,38 @@
         <v>0</v>
       </c>
       <c r="D16">
-        <v>0.20026368005563511</v>
+        <v>0.1938115037899574</v>
       </c>
       <c r="E16">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="F16">
-        <v>10000</v>
+        <v>250</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>5000</v>
+        <v>500</v>
       </c>
       <c r="B17">
-        <v>12</v>
+        <v>356</v>
       </c>
       <c r="C17">
-        <v>2.3999999999999998E-3</v>
+        <v>0.71199999999999997</v>
       </c>
       <c r="D17">
-        <v>0.20081901347689871</v>
+        <v>0.1860307443971965</v>
       </c>
       <c r="E17">
         <v>50</v>
       </c>
       <c r="F17">
-        <v>5000</v>
+        <v>500</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>2500</v>
+        <v>500</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -825,13 +2027,13 @@
         <v>0</v>
       </c>
       <c r="D18">
-        <v>0.20114639184815269</v>
+        <v>0.19622981049565191</v>
       </c>
       <c r="E18">
         <v>100</v>
       </c>
       <c r="F18">
-        <v>2500</v>
+        <v>500</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -856,27 +2058,27 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>5000</v>
+        <v>500</v>
       </c>
       <c r="B20">
-        <v>501</v>
+        <v>0</v>
       </c>
       <c r="C20">
-        <v>0.1002</v>
+        <v>0</v>
       </c>
       <c r="D20">
-        <v>0.20160217448352971</v>
+        <v>0.2252493770949936</v>
       </c>
       <c r="E20">
-        <v>100</v>
+        <v>350</v>
       </c>
       <c r="F20">
-        <v>5000</v>
+        <v>500</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>50</v>
+        <v>500</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -885,38 +2087,38 @@
         <v>0</v>
       </c>
       <c r="D21">
-        <v>0.20246057617065999</v>
+        <v>0.21128361196510481</v>
       </c>
       <c r="E21">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="F21">
-        <v>50</v>
+        <v>500</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>125</v>
+        <v>1250</v>
       </c>
       <c r="B22">
-        <v>0</v>
+        <v>116</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>9.2799999999999994E-2</v>
       </c>
       <c r="D22">
-        <v>0.2033428866265182</v>
+        <v>0.20946377353589199</v>
       </c>
       <c r="E22">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="F22">
-        <v>125</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>2500</v>
+        <v>1250</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -925,13 +2127,13 @@
         <v>0</v>
       </c>
       <c r="D23">
-        <v>0.20559030160475991</v>
+        <v>0.19976847983663551</v>
       </c>
       <c r="E23">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="F23">
-        <v>2500</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -956,22 +2158,22 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>125</v>
+        <v>1250</v>
       </c>
       <c r="B25">
-        <v>74</v>
+        <v>0</v>
       </c>
       <c r="C25">
-        <v>0.59199999999999997</v>
+        <v>0</v>
       </c>
       <c r="D25">
-        <v>0.2079526988098267</v>
+        <v>0.20754198563472151</v>
       </c>
       <c r="E25">
-        <v>50</v>
+        <v>350</v>
       </c>
       <c r="F25">
-        <v>125</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -979,16 +2181,16 @@
         <v>1250</v>
       </c>
       <c r="B26">
-        <v>116</v>
+        <v>0</v>
       </c>
       <c r="C26">
-        <v>9.2799999999999994E-2</v>
+        <v>0</v>
       </c>
       <c r="D26">
-        <v>0.20946377353589199</v>
+        <v>0.19541331908026269</v>
       </c>
       <c r="E26">
-        <v>50</v>
+        <v>500</v>
       </c>
       <c r="F26">
         <v>1250</v>
@@ -996,27 +2198,27 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>125</v>
+        <v>2500</v>
       </c>
       <c r="B27">
-        <v>3</v>
+        <v>1606</v>
       </c>
       <c r="C27">
-        <v>2.4E-2</v>
+        <v>0.64239999999999997</v>
       </c>
       <c r="D27">
-        <v>0.23124964311832219</v>
+        <v>0.19902327845823481</v>
       </c>
       <c r="E27">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="F27">
-        <v>125</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>50</v>
+        <v>2500</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -1025,19 +2227,381 @@
         <v>0</v>
       </c>
       <c r="D28">
-        <v>0.2441999009867436</v>
+        <v>0.20114639184815269</v>
       </c>
       <c r="E28">
         <v>100</v>
       </c>
       <c r="F28">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>2500</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0.20559030160475991</v>
+      </c>
+      <c r="E29">
+        <v>200</v>
+      </c>
+      <c r="F29">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>2500</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0.20109029954042129</v>
+      </c>
+      <c r="E30">
+        <v>350</v>
+      </c>
+      <c r="F30">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>2500</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0.20539094844824651</v>
+      </c>
+      <c r="E31">
+        <v>500</v>
+      </c>
+      <c r="F31">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>5000</v>
+      </c>
+      <c r="B32">
+        <v>12</v>
+      </c>
+      <c r="C32">
+        <v>2.3999999999999998E-3</v>
+      </c>
+      <c r="D32">
+        <v>0.20081901347689871</v>
+      </c>
+      <c r="E32">
         <v>50</v>
+      </c>
+      <c r="F32">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>5000</v>
+      </c>
+      <c r="B33">
+        <v>501</v>
+      </c>
+      <c r="C33">
+        <v>0.1002</v>
+      </c>
+      <c r="D33">
+        <v>0.20160217448352971</v>
+      </c>
+      <c r="E33">
+        <v>100</v>
+      </c>
+      <c r="F33">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>5000</v>
+      </c>
+      <c r="B34">
+        <v>3865</v>
+      </c>
+      <c r="C34">
+        <v>0.77300000000000002</v>
+      </c>
+      <c r="D34">
+        <v>0.19916207111113179</v>
+      </c>
+      <c r="E34">
+        <v>200</v>
+      </c>
+      <c r="F34">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>5000</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0.20248256527720221</v>
+      </c>
+      <c r="E35">
+        <v>350</v>
+      </c>
+      <c r="F35">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>5000</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0.19642075876852411</v>
+      </c>
+      <c r="E36">
+        <v>500</v>
+      </c>
+      <c r="F36">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>7500</v>
+      </c>
+      <c r="B37">
+        <v>776</v>
+      </c>
+      <c r="C37">
+        <v>0.10346666666666671</v>
+      </c>
+      <c r="D37">
+        <v>0.19978617109152219</v>
+      </c>
+      <c r="E37">
+        <v>50</v>
+      </c>
+      <c r="F37">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>7500</v>
+      </c>
+      <c r="B38">
+        <v>5</v>
+      </c>
+      <c r="C38">
+        <v>6.6666666666666664E-4</v>
+      </c>
+      <c r="D38">
+        <v>0.19711089904670601</v>
+      </c>
+      <c r="E38">
+        <v>100</v>
+      </c>
+      <c r="F38">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>7500</v>
+      </c>
+      <c r="B39">
+        <v>0</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>0.19706118521253521</v>
+      </c>
+      <c r="E39">
+        <v>200</v>
+      </c>
+      <c r="F39">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>7500</v>
+      </c>
+      <c r="B40">
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>0.2002509615684771</v>
+      </c>
+      <c r="E40">
+        <v>350</v>
+      </c>
+      <c r="F40">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>7500</v>
+      </c>
+      <c r="B41">
+        <v>0</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>0.198604481137239</v>
+      </c>
+      <c r="E41">
+        <v>500</v>
+      </c>
+      <c r="F41">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>10000</v>
+      </c>
+      <c r="B42">
+        <v>2536</v>
+      </c>
+      <c r="C42">
+        <v>0.25359999999999999</v>
+      </c>
+      <c r="D42">
+        <v>0.19778613638600959</v>
+      </c>
+      <c r="E42">
+        <v>50</v>
+      </c>
+      <c r="F42">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>10000</v>
+      </c>
+      <c r="B43">
+        <v>0</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>0.19817352595832419</v>
+      </c>
+      <c r="E43">
+        <v>100</v>
+      </c>
+      <c r="F43">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>10000</v>
+      </c>
+      <c r="B44">
+        <v>0</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>0.20026368005563511</v>
+      </c>
+      <c r="E44">
+        <v>200</v>
+      </c>
+      <c r="F44">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>10000</v>
+      </c>
+      <c r="B45">
+        <v>0</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>0.19565811314984841</v>
+      </c>
+      <c r="E45">
+        <v>350</v>
+      </c>
+      <c r="F45">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>10000</v>
+      </c>
+      <c r="B46">
+        <v>0</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>0.20210721228199419</v>
+      </c>
+      <c r="E46">
+        <v>500</v>
+      </c>
+      <c r="F46">
+        <v>10000</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>